<commit_message>
Novos testes com o UiPath
</commit_message>
<xml_diff>
--- a/ROBO_OCR/ID/Registro.xlsx
+++ b/ROBO_OCR/ID/Registro.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Alex Silva "</t>
+  </si>
+  <si>
+    <t>Liliane Santoé</t>
+  </si>
+  <si>
+    <t>Sueli Santos '4</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -439,6 +445,358 @@
       </c>
       <c r="C6" s="3">
         <v>38050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>123956789</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>123956789</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>123956789</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>123956789</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>123956789</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>123956789</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>123956789</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>123956789</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>123956789</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>123956789</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>123956789</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>123956789</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>123956789</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>123956789</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>123956789</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>123956789</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>123956789</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>123956789</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>123956789</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>123956789</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>123956789</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>123956789</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>123956789</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>123956789</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>123956789</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="3">
+        <v>31569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>122456789</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="3">
+        <v>29871</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>122456789</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="3">
+        <v>29871</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>122456789</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="3">
+        <v>29871</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>122456789</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3">
+        <v>29871</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>122456789</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3">
+        <v>29871</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>122456789</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3">
+        <v>29871</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>123956789</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="3">
+        <v>31569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>